<commit_message>
Details for xlsx package
</commit_message>
<xml_diff>
--- a/XLSX/xlsx/data.xlsx
+++ b/XLSX/xlsx/data.xlsx
@@ -1,19 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21231"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zerocho\WebstormProjects\nodejs-crawler\2.xlsx-parsing-example\xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\Documents\project\node-crawler\XLSX\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12801383-EAC9-40A5-BE04-090991985550}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2625" yWindow="3240" windowWidth="21600" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8040" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="영화목록" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet3" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
@@ -108,7 +110,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1069,11 +1071,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1173,12 +1175,53 @@
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="B10" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="B11" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="B3" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="B2" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="B8" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="B10" r:id="rId1"/>
+    <hyperlink ref="B11" r:id="rId2"/>
+    <hyperlink ref="B3" r:id="rId3"/>
+    <hyperlink ref="B2" r:id="rId4"/>
+    <hyperlink ref="B8" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <phoneticPr fontId="18" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <phoneticPr fontId="18" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I17" sqref="I17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <phoneticPr fontId="18" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>